<commit_message>
Updates to functionality and dependency repairs
</commit_message>
<xml_diff>
--- a/latexutils/tables.xlsx
+++ b/latexutils/tables.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsievers/programming/python/latexutils/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsievers/programming/GitHub/latexutils/latexutils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDD049E-632B-C543-BB88-2D019BBAA194}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7056CA01-AC32-5346-9459-1B3E16690715}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9640" yWindow="5520" windowWidth="23960" windowHeight="15400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1600" yWindow="10420" windowWidth="23960" windowHeight="15400" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$2:$J$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$A$2:$J$17</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="39">
   <si>
     <t>t (h)</t>
   </si>
@@ -72,6 +74,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>x</t>
     </r>
@@ -80,6 +83,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> (1/min)</t>
     </r>
@@ -94,6 +98,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>g</t>
     </r>
@@ -102,6 +107,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> (1/min)</t>
     </r>
@@ -126,6 +132,87 @@
   </si>
   <si>
     <t>%.2e</t>
+  </si>
+  <si>
+    <t>Abs. Pressure</t>
+  </si>
+  <si>
+    <t>(kPa)</t>
+  </si>
+  <si>
+    <t>Temp.</t>
+  </si>
+  <si>
+    <t>(°C)</t>
+  </si>
+  <si>
+    <t>(g/L)</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>(h)</t>
+  </si>
+  <si>
+    <r>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>x</t>
+    </r>
+  </si>
+  <si>
+    <t>(1/min)</t>
+  </si>
+  <si>
+    <r>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>g</t>
+    </r>
+  </si>
+  <si>
+    <t>%.1fS</t>
+  </si>
+  <si>
+    <t>%.2fS</t>
+  </si>
+  <si>
+    <t>%iS</t>
+  </si>
+  <si>
+    <t>Starting</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>Liquor</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Starting Total</t>
+  </si>
+  <si>
+    <t>Conc.</t>
   </si>
 </sst>
 </file>
@@ -163,6 +250,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -175,12 +263,14 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <vertAlign val="subscript"/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -191,7 +281,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -228,6 +318,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -254,7 +362,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -340,6 +448,33 @@
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="23">
@@ -707,7 +842,7 @@
   </sheetPr>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -1214,7 +1349,7 @@
       <c r="H16" s="28"/>
     </row>
   </sheetData>
-  <sortState ref="A3:J15">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J15">
     <sortCondition ref="B3:B15"/>
     <sortCondition ref="H3:H15"/>
     <sortCondition ref="D3:D15"/>
@@ -1229,4 +1364,565 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F3FD5FF-74F3-8B40-A70B-FAA58E0D2E6F}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="8.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="3"/>
+    <col min="8" max="8" width="6" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="3"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="5" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="5" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="36"/>
+      <c r="B3" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+    </row>
+    <row r="4" spans="1:10" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="35"/>
+      <c r="G4" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="9">
+        <v>8</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="12">
+        <v>81.276737967914443</v>
+      </c>
+      <c r="E5" s="10">
+        <v>98.694725433527296</v>
+      </c>
+      <c r="F5" s="11">
+        <v>3.77999999999999</v>
+      </c>
+      <c r="G5" s="12">
+        <v>521.73844775304894</v>
+      </c>
+      <c r="H5" s="12">
+        <v>24</v>
+      </c>
+      <c r="I5" s="13">
+        <v>5.8657565937631899E-5</v>
+      </c>
+      <c r="J5" s="13">
+        <v>2.0470019606263701E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="14">
+        <v>9</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="17">
+        <v>81.276737967914443</v>
+      </c>
+      <c r="E6" s="15">
+        <v>99</v>
+      </c>
+      <c r="F6" s="16">
+        <v>3.85</v>
+      </c>
+      <c r="G6" s="17">
+        <v>520.99637944745302</v>
+      </c>
+      <c r="H6" s="17">
+        <v>6</v>
+      </c>
+      <c r="I6" s="18">
+        <v>4.8405466942801301E-4</v>
+      </c>
+      <c r="J6" s="18">
+        <v>1.59472086514149E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="14">
+        <v>13</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="17">
+        <v>81.276737967914443</v>
+      </c>
+      <c r="E7" s="15">
+        <v>95.724354501045497</v>
+      </c>
+      <c r="F7" s="16">
+        <v>2.91</v>
+      </c>
+      <c r="G7" s="17">
+        <v>100.912000947233</v>
+      </c>
+      <c r="H7" s="17">
+        <v>24</v>
+      </c>
+      <c r="I7" s="18">
+        <v>1.45938319822185E-6</v>
+      </c>
+      <c r="J7" s="18">
+        <v>5.6514708655219202E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="14">
+        <v>12</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="17">
+        <v>81.276737967914443</v>
+      </c>
+      <c r="E8" s="15">
+        <v>95.300955414012094</v>
+      </c>
+      <c r="F8" s="16">
+        <v>4.78</v>
+      </c>
+      <c r="G8" s="17">
+        <v>101.23614970359</v>
+      </c>
+      <c r="H8" s="17">
+        <v>24</v>
+      </c>
+      <c r="I8" s="18">
+        <v>5.6581763383167998E-5</v>
+      </c>
+      <c r="J8" s="18">
+        <v>1.5280269238531598E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="14">
+        <v>15</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="17">
+        <v>81.276737967914443</v>
+      </c>
+      <c r="E9" s="15">
+        <v>96.836390927284896</v>
+      </c>
+      <c r="F9" s="16">
+        <v>4.79</v>
+      </c>
+      <c r="G9" s="17">
+        <v>102.025515916893</v>
+      </c>
+      <c r="H9" s="17">
+        <v>24</v>
+      </c>
+      <c r="I9" s="18">
+        <v>5.5726830521001501E-5</v>
+      </c>
+      <c r="J9" s="18">
+        <v>1.89576175566755E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="14">
+        <v>18</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="17">
+        <v>81.276737967914443</v>
+      </c>
+      <c r="E10" s="15">
+        <v>96.715593220338604</v>
+      </c>
+      <c r="F10" s="16">
+        <v>4.78</v>
+      </c>
+      <c r="G10" s="17">
+        <v>102.71676875440301</v>
+      </c>
+      <c r="H10" s="17">
+        <v>24</v>
+      </c>
+      <c r="I10" s="18">
+        <v>5.2742633723280799E-5</v>
+      </c>
+      <c r="J10" s="18">
+        <v>1.4011394750205201E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="14">
+        <v>14</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="17">
+        <v>30.478776737967912</v>
+      </c>
+      <c r="E11" s="15">
+        <v>69.989169675088903</v>
+      </c>
+      <c r="F11" s="16">
+        <v>4.82</v>
+      </c>
+      <c r="G11" s="17">
+        <v>101.200513429152</v>
+      </c>
+      <c r="H11" s="17">
+        <v>24</v>
+      </c>
+      <c r="I11" s="18">
+        <v>2.3963411306559399E-5</v>
+      </c>
+      <c r="J11" s="18">
+        <v>2.3456872335958999E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="14">
+        <v>17</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="17">
+        <v>81.276737967914443</v>
+      </c>
+      <c r="E12" s="15">
+        <v>100.043055555555</v>
+      </c>
+      <c r="F12" s="16">
+        <v>3.1699999999999902</v>
+      </c>
+      <c r="G12" s="17">
+        <v>533.12094823567702</v>
+      </c>
+      <c r="H12" s="17">
+        <v>6</v>
+      </c>
+      <c r="I12" s="18">
+        <v>7.1454005299017404E-4</v>
+      </c>
+      <c r="J12" s="18">
+        <v>2.3596606380004299E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="14">
+        <v>16</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="17">
+        <v>81.276737967914443</v>
+      </c>
+      <c r="E13" s="15">
+        <v>99.499336870026497</v>
+      </c>
+      <c r="F13" s="16">
+        <v>4.78</v>
+      </c>
+      <c r="G13" s="17">
+        <v>549.06534196088398</v>
+      </c>
+      <c r="H13" s="17">
+        <v>6</v>
+      </c>
+      <c r="I13" s="18">
+        <v>1.0593504150693601E-3</v>
+      </c>
+      <c r="J13" s="18">
+        <v>3.20413319468579E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="14">
+        <v>22</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="17">
+        <v>47.411430481283425</v>
+      </c>
+      <c r="E14" s="15">
+        <v>83.442613636363603</v>
+      </c>
+      <c r="F14" s="16">
+        <v>2.93</v>
+      </c>
+      <c r="G14" s="17">
+        <v>562.32010046170001</v>
+      </c>
+      <c r="H14" s="17">
+        <v>6</v>
+      </c>
+      <c r="I14" s="18">
+        <v>6.8101129039107501E-5</v>
+      </c>
+      <c r="J14" s="18">
+        <v>8.3913467005751895E-13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="14">
+        <v>20</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="17">
+        <v>47.411430481283425</v>
+      </c>
+      <c r="E15" s="15">
+        <v>85.282981530342994</v>
+      </c>
+      <c r="F15" s="16">
+        <v>4.87</v>
+      </c>
+      <c r="G15" s="17">
+        <v>546.15685984341405</v>
+      </c>
+      <c r="H15" s="17">
+        <v>6</v>
+      </c>
+      <c r="I15" s="18">
+        <v>2.2525340437642801E-4</v>
+      </c>
+      <c r="J15" s="18">
+        <v>7.8328492400560795E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="14">
+        <v>21</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="17">
+        <v>30.478776737967912</v>
+      </c>
+      <c r="E16" s="15">
+        <v>73.520633397312807</v>
+      </c>
+      <c r="F16" s="16">
+        <v>2.72</v>
+      </c>
+      <c r="G16" s="17">
+        <v>553.15405005090895</v>
+      </c>
+      <c r="H16" s="17">
+        <v>6</v>
+      </c>
+      <c r="I16" s="18">
+        <v>3.0197012976197901E-5</v>
+      </c>
+      <c r="J16" s="18">
+        <v>2.0424681797937802E-6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
+        <v>19</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="24">
+        <v>30.478776737967912</v>
+      </c>
+      <c r="E17" s="22">
+        <v>73.458673469387705</v>
+      </c>
+      <c r="F17" s="23">
+        <v>5.04</v>
+      </c>
+      <c r="G17" s="24">
+        <v>560.77707653974403</v>
+      </c>
+      <c r="H17" s="24">
+        <v>6</v>
+      </c>
+      <c r="I17" s="26">
+        <v>1.6529889324851899E-4</v>
+      </c>
+      <c r="J17" s="26">
+        <v>6.9063338741239295E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="27"/>
+      <c r="F18" s="4"/>
+      <c r="H18" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup scale="80" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
 </file>
</xml_diff>